<commit_message>
Correlation Column Logic and Data Gen.
</commit_message>
<xml_diff>
--- a/config/table_config.xlsx
+++ b/config/table_config.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="21">
   <si>
     <t>DOMAIN</t>
   </si>
@@ -25,6 +25,9 @@
     <t>ROWS</t>
   </si>
   <si>
+    <t>GEN_ORDER</t>
+  </si>
+  <si>
     <t>COLUMN_ORDER</t>
   </si>
   <si>
@@ -37,22 +40,43 @@
     <t>LIFNR, BU_GROUP, KTOKK, NAME_FIRST, NAME_FIRST_P, NAME_LAST_P, BPEXT, STREET, POST_CODE1, CITY1, COUNTRY, REGION, LANGU_CORR, TELNR_LONG, SMTP_ADDR</t>
   </si>
   <si>
+    <t>S_LFA1_TEXT</t>
+  </si>
+  <si>
+    <t>LIFNR,TDSPRAS</t>
+  </si>
+  <si>
+    <t>S_SUPPL_ADDR</t>
+  </si>
+  <si>
+    <t>LIFNR</t>
+  </si>
+  <si>
+    <t>S_LFM1_TEXT</t>
+  </si>
+  <si>
+    <t>S_SUPPL_WITH_TAX</t>
+  </si>
+  <si>
+    <t>LIFNR,BUKRS</t>
+  </si>
+  <si>
     <t>S_ROLES</t>
   </si>
   <si>
-    <t>S_LFA1_TEXT</t>
-  </si>
-  <si>
-    <t>S_LFM1_TEXT</t>
-  </si>
-  <si>
-    <t>S_SUPPL_ADDR</t>
-  </si>
-  <si>
-    <t>S_SUPPL_WITH_TAX</t>
+    <t>LIFNR,BP_ROLE</t>
   </si>
   <si>
     <t>S_ADDR_USAGE</t>
+  </si>
+  <si>
+    <t>LIFNR, ADR_KIND</t>
+  </si>
+  <si>
+    <t>S_SUPPL_PARTNER</t>
+  </si>
+  <si>
+    <t>LIFNR,EKORG,PARVW,LIFN2,DEFPA</t>
   </si>
 </sst>
 </file>
@@ -132,11 +156,11 @@
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -452,16 +476,17 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" style="6" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="6" width="23.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="7" width="44.86214285714286" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="8" width="141.57642857142858" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="6" width="16.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="7" width="108.57642857142856" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="8" width="141.57642857142858" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
@@ -474,95 +499,155 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="3">
+        <v>15</v>
+      </c>
+      <c r="D2" s="3">
+        <v>1</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
+      <c r="A3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="3">
+        <v>5</v>
+      </c>
+      <c r="D3" s="3">
+        <v>2</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
+      <c r="A4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="3">
+        <v>5</v>
+      </c>
+      <c r="D4" s="3">
+        <v>3</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
+      <c r="A5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="3">
+        <v>5</v>
+      </c>
+      <c r="D5" s="3">
         <v>4</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="4">
+      <c r="E5" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
+      <c r="A6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="3">
+        <v>5</v>
+      </c>
+      <c r="D6" s="3">
+        <v>5</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
+      <c r="A7" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="C7" s="3">
+        <v>5</v>
+      </c>
+      <c r="D7" s="3">
         <v>6</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
-      <c r="A3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="3" t="s">
+      <c r="E7" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
+      <c r="A8" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="3">
+        <v>5</v>
+      </c>
+      <c r="D8" s="3">
         <v>7</v>
       </c>
-      <c r="C3" s="4">
-        <v>5</v>
-      </c>
-      <c r="D3" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
-      <c r="A4" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="3" t="s">
+      <c r="E8" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
+      <c r="A9" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="3">
+        <v>5</v>
+      </c>
+      <c r="D9" s="3">
         <v>8</v>
       </c>
-      <c r="C4" s="4">
-        <v>5</v>
-      </c>
-      <c r="D4" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
-      <c r="A5" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="4">
-        <v>5</v>
-      </c>
-      <c r="D5" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
-      <c r="A6" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="4">
-        <v>5</v>
-      </c>
-      <c r="D6" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
-      <c r="A7" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="4">
-        <v>5</v>
-      </c>
-      <c r="D7" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
-      <c r="A8" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="4">
-        <v>5</v>
-      </c>
-      <c r="D8" s="4"/>
+      <c r="E9" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add more table and descriptions
</commit_message>
<xml_diff>
--- a/config/table_config.xlsx
+++ b/config/table_config.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="27">
   <si>
     <t>DOMAIN</t>
   </si>
@@ -77,6 +77,24 @@
   </si>
   <si>
     <t>LIFNR,EKORG,PARVW,LIFN2,DEFPA</t>
+  </si>
+  <si>
+    <t>S_SUPPL_COMPANY</t>
+  </si>
+  <si>
+    <t>LIFNR,BUKRS,AKONT,ZTERM1,ZWELS_01</t>
+  </si>
+  <si>
+    <t>S_SUPP_BANK</t>
+  </si>
+  <si>
+    <t>LIFNR,BANKS,BANKL,BANKN,IBAN,BKONT,BKREF,KOINH,EBPP_ACCNAME</t>
+  </si>
+  <si>
+    <t>S_SUPPL_PURCHASING</t>
+  </si>
+  <si>
+    <t>LIFNR,EKORG,WAERS,ZTERM,INCO1,INCO2,KALKS,VSBED,WEBRE,KZAUT,BSTAE,KZRET</t>
   </si>
 </sst>
 </file>
@@ -148,7 +166,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -163,6 +181,12 @@
       <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -476,17 +500,17 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="6" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="6" width="16.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="7" width="108.57642857142856" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="8" width="141.57642857142858" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="8" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="8" width="28.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="9" width="108.57642857142856" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="10" width="141.57642857142858" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
@@ -642,12 +666,56 @@
         <v>20</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="5"/>
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="17.25">
+      <c r="A10" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="6">
+        <v>5</v>
+      </c>
+      <c r="D10" s="6">
+        <v>9</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="17.25">
+      <c r="A11" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="6">
+        <v>5</v>
+      </c>
+      <c r="D11" s="6">
+        <v>10</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
+      <c r="A12" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="3">
+        <v>5</v>
+      </c>
+      <c r="D12" s="3">
+        <v>11</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>26</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Vendor and Equipment - table_confing adjustments.
</commit_message>
<xml_diff>
--- a/config/table_config.xlsx
+++ b/config/table_config.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="36">
   <si>
     <t>DOMAIN</t>
   </si>
@@ -40,27 +40,57 @@
     <t>LIFNR, BU_GROUP, KTOKK, NAME_FIRST, NAME_FIRST_P, NAME_LAST_P, BPEXT, STREET, POST_CODE1, CITY1, COUNTRY, REGION, LANGU_CORR, TELNR_LONG, SMTP_ADDR</t>
   </si>
   <si>
+    <t>S_SUPPL_ADDR</t>
+  </si>
+  <si>
+    <t>LIFNR</t>
+  </si>
+  <si>
+    <t>S_SUPPL_COMPANY</t>
+  </si>
+  <si>
+    <t>LIFNR,BUKRS,AKONT,ZTERM1,ZWELS_01</t>
+  </si>
+  <si>
+    <t>S_SUPPL_PURCHASING</t>
+  </si>
+  <si>
+    <t>LIFNR,EKORG,WAERS,ZTERM,INCO1,INCO2,KALKS,VSBED,WEBRE,KZAUT,BSTAE,KZRET</t>
+  </si>
+  <si>
+    <t>S_SUPP_BANK</t>
+  </si>
+  <si>
+    <t>LIFNR,BANKS,BANKL,BANKN,IBAN,BKONT,BKREF,KOINH,EBPP_ACCNAME</t>
+  </si>
+  <si>
+    <t>S_SUPPL_PARTNER</t>
+  </si>
+  <si>
+    <t>LIFNR,EKORG,PARVW,LIFN2,DEFPA</t>
+  </si>
+  <si>
+    <t>S_SUPPL_TAXNUMBERS</t>
+  </si>
+  <si>
+    <t>TAXTYPE,TAXNUM</t>
+  </si>
+  <si>
+    <t>S_SUPPL_WITH_TAX</t>
+  </si>
+  <si>
+    <t>LIFNR,BUKRS</t>
+  </si>
+  <si>
     <t>S_LFA1_TEXT</t>
   </si>
   <si>
     <t>LIFNR,TDSPRAS</t>
   </si>
   <si>
-    <t>S_SUPPL_ADDR</t>
-  </si>
-  <si>
-    <t>LIFNR</t>
-  </si>
-  <si>
     <t>S_LFM1_TEXT</t>
   </si>
   <si>
-    <t>S_SUPPL_WITH_TAX</t>
-  </si>
-  <si>
-    <t>LIFNR,BUKRS</t>
-  </si>
-  <si>
     <t>S_ROLES</t>
   </si>
   <si>
@@ -70,31 +100,7 @@
     <t>S_ADDR_USAGE</t>
   </si>
   <si>
-    <t>LIFNR, ADR_KIND</t>
-  </si>
-  <si>
-    <t>S_SUPPL_PARTNER</t>
-  </si>
-  <si>
-    <t>LIFNR,EKORG,PARVW,LIFN2,DEFPA</t>
-  </si>
-  <si>
-    <t>S_SUPPL_COMPANY</t>
-  </si>
-  <si>
-    <t>LIFNR,BUKRS,AKONT,ZTERM1,ZWELS_01</t>
-  </si>
-  <si>
-    <t>S_SUPP_BANK</t>
-  </si>
-  <si>
-    <t>LIFNR,BANKS,BANKL,BANKN,IBAN,BKONT,BKREF,KOINH,EBPP_ACCNAME</t>
-  </si>
-  <si>
-    <t>S_SUPPL_PURCHASING</t>
-  </si>
-  <si>
-    <t>LIFNR,EKORG,WAERS,ZTERM,INCO1,INCO2,KALKS,VSBED,WEBRE,KZAUT,BSTAE,KZRET</t>
+    <t>LIFNR,ADR_KIND</t>
   </si>
   <si>
     <t>equipment</t>
@@ -123,7 +129,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -141,12 +147,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -193,7 +193,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -208,12 +208,6 @@
       <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -527,17 +521,17 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="8" width="25.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="8" width="28.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="9" width="108.57642857142856" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="10" width="141.57642857142858" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="6" width="25.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="6" width="26.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="7" width="20.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="8" width="141.57642857142858" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
@@ -565,7 +559,7 @@
         <v>6</v>
       </c>
       <c r="C2" s="3">
-        <v>15</v>
+        <v>100</v>
       </c>
       <c r="D2" s="3">
         <v>1</v>
@@ -574,7 +568,7 @@
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
       <c r="A3" s="4" t="s">
         <v>5</v>
       </c>
@@ -582,7 +576,7 @@
         <v>8</v>
       </c>
       <c r="C3" s="3">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="D3" s="3">
         <v>2</v>
@@ -591,7 +585,7 @@
         <v>9</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25">
       <c r="A4" s="4" t="s">
         <v>5</v>
       </c>
@@ -599,7 +593,7 @@
         <v>10</v>
       </c>
       <c r="C4" s="3">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="D4" s="3">
         <v>3</v>
@@ -616,13 +610,13 @@
         <v>12</v>
       </c>
       <c r="C5" s="3">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="D5" s="3">
         <v>4</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
@@ -630,16 +624,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C6" s="3">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="D6" s="3">
         <v>5</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
@@ -647,16 +641,16 @@
         <v>5</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C7" s="3">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="D7" s="3">
         <v>6</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
@@ -664,16 +658,16 @@
         <v>5</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C8" s="3">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="D8" s="3">
         <v>7</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
@@ -681,16 +675,16 @@
         <v>5</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C9" s="3">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="D9" s="3">
         <v>8</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
@@ -698,16 +692,16 @@
         <v>5</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C10" s="3">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="D10" s="3">
         <v>9</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
@@ -715,16 +709,16 @@
         <v>5</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C11" s="3">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="D11" s="3">
         <v>10</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
@@ -735,7 +729,7 @@
         <v>25</v>
       </c>
       <c r="C12" s="3">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="D12" s="3">
         <v>11</v>
@@ -744,63 +738,80 @@
         <v>26</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="C13" s="3">
+        <v>100</v>
+      </c>
+      <c r="D13" s="3">
+        <v>12</v>
+      </c>
+      <c r="E13" s="5" t="s">
         <v>28</v>
-      </c>
-      <c r="C13" s="6">
-        <v>15</v>
-      </c>
-      <c r="D13" s="6">
-        <v>12</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>29</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="17.25">
       <c r="A14" s="4" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C14" s="6">
-        <v>5</v>
-      </c>
-      <c r="D14" s="6">
-        <v>13</v>
-      </c>
-      <c r="E14" s="7" t="s">
+      <c r="C14" s="3">
+        <v>100</v>
+      </c>
+      <c r="D14" s="3">
+        <v>12</v>
+      </c>
+      <c r="E14" s="5" t="s">
         <v>31</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="17.25">
       <c r="A15" s="4" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C15" s="6">
-        <v>5</v>
-      </c>
-      <c r="D15" s="6">
+      <c r="C15" s="3">
+        <v>100</v>
+      </c>
+      <c r="D15" s="3">
+        <v>13</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="17.25">
+      <c r="A16" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" s="3">
+        <v>100</v>
+      </c>
+      <c r="D16" s="3">
         <v>14</v>
       </c>
-      <c r="E15" s="7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="5"/>
+      <c r="E16" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
+      <c r="A17" s="4"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Working on employee logic
</commit_message>
<xml_diff>
--- a/config/table_config.xlsx
+++ b/config/table_config.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>DOMAIN</t>
   </si>
@@ -31,101 +31,16 @@
     <t>COLUMN_ORDER</t>
   </si>
   <si>
-    <t>vendor</t>
-  </si>
-  <si>
-    <t>S_SUPPL_GEN</t>
-  </si>
-  <si>
-    <t>LIFNR, BU_GROUP, KTOKK, NAME_FIRST, NAME_FIRST_P, NAME_LAST_P, BPEXT, STREET, POST_CODE1, CITY1, COUNTRY, REGION, LANGU_CORR, TELNR_LONG, SMTP_ADDR</t>
-  </si>
-  <si>
-    <t>S_SUPPL_ADDR</t>
-  </si>
-  <si>
-    <t>LIFNR</t>
-  </si>
-  <si>
-    <t>S_SUPPL_COMPANY</t>
-  </si>
-  <si>
-    <t>LIFNR,BUKRS,AKONT,ZTERM1,ZWELS_01</t>
-  </si>
-  <si>
-    <t>S_SUPPL_PURCHASING</t>
-  </si>
-  <si>
-    <t>LIFNR,EKORG,WAERS,ZTERM,INCO1,INCO2,KALKS,VSBED,WEBRE,KZAUT,BSTAE,KZRET</t>
-  </si>
-  <si>
-    <t>S_SUPP_BANK</t>
-  </si>
-  <si>
-    <t>LIFNR,BANKS,BANKL,BANKN,IBAN,BKONT,BKREF,KOINH,EBPP_ACCNAME</t>
-  </si>
-  <si>
-    <t>S_SUPPL_PARTNER</t>
-  </si>
-  <si>
-    <t>LIFNR,EKORG,PARVW,LIFN2,DEFPA</t>
-  </si>
-  <si>
-    <t>S_SUPPL_TAXNUMBERS</t>
-  </si>
-  <si>
-    <t>TAXTYPE,TAXNUM</t>
-  </si>
-  <si>
-    <t>S_SUPPL_WITH_TAX</t>
-  </si>
-  <si>
-    <t>LIFNR,BUKRS</t>
-  </si>
-  <si>
-    <t>S_LFA1_TEXT</t>
-  </si>
-  <si>
-    <t>LIFNR,TDSPRAS</t>
-  </si>
-  <si>
-    <t>S_LFM1_TEXT</t>
-  </si>
-  <si>
-    <t>S_ROLES</t>
-  </si>
-  <si>
-    <t>LIFNR,BP_ROLE</t>
-  </si>
-  <si>
-    <t>S_ADDR_USAGE</t>
-  </si>
-  <si>
-    <t>LIFNR,ADR_KIND</t>
-  </si>
-  <si>
-    <t>equipment</t>
-  </si>
-  <si>
-    <t>S_EQUI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">40,000
-</t>
-  </si>
-  <si>
-    <t>EQUNR,NRANGE_IND,EQTYP,DATAB,EQKTX,BRGEW,GEWEI,MATNR,GERNR</t>
-  </si>
-  <si>
-    <t>S_IHPA</t>
-  </si>
-  <si>
-    <t>EQUNR,PARVW</t>
-  </si>
-  <si>
-    <t>S_TEXTS_EQUI</t>
-  </si>
-  <si>
-    <t>EQUNR,SPRAS,TEXT_DESCR</t>
+    <t>employee</t>
+  </si>
+  <si>
+    <t>S_EMPLOYEE</t>
+  </si>
+  <si>
+    <t>PERNR</t>
+  </si>
+  <si>
+    <t>S_PA0000</t>
   </si>
 </sst>
 </file>
@@ -563,7 +478,7 @@
         <v>6</v>
       </c>
       <c r="C2" s="3">
-        <v>40000</v>
+        <v>30</v>
       </c>
       <c r="D2" s="3">
         <v>1</v>
@@ -580,235 +495,103 @@
         <v>8</v>
       </c>
       <c r="C3" s="3">
-        <v>40000</v>
+        <v>15</v>
       </c>
       <c r="D3" s="3">
         <v>2</v>
       </c>
-      <c r="E3" s="5" t="s">
-        <v>9</v>
-      </c>
+      <c r="E3" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
-      <c r="A4" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="3">
-        <v>40000</v>
-      </c>
-      <c r="D4" s="3">
-        <v>3</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>11</v>
-      </c>
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
-      <c r="A5" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="3">
-        <v>40000</v>
-      </c>
-      <c r="D5" s="3">
-        <v>4</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>13</v>
-      </c>
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
-      <c r="A6" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="3">
-        <v>40000</v>
-      </c>
-      <c r="D6" s="3">
-        <v>5</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>15</v>
-      </c>
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
-      <c r="A7" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="3">
-        <v>40000</v>
-      </c>
-      <c r="D7" s="3">
-        <v>6</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>17</v>
-      </c>
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
-      <c r="A8" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" s="3">
-        <v>40000</v>
-      </c>
-      <c r="D8" s="3">
-        <v>7</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>19</v>
-      </c>
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
-      <c r="A9" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" s="3">
-        <v>40000</v>
-      </c>
-      <c r="D9" s="3">
-        <v>8</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>21</v>
-      </c>
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
-      <c r="A10" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10" s="3">
-        <v>40000</v>
-      </c>
-      <c r="D10" s="3">
-        <v>9</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>23</v>
-      </c>
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
-      <c r="A11" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C11" s="3">
-        <v>40000</v>
-      </c>
-      <c r="D11" s="3">
-        <v>10</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>9</v>
-      </c>
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
-      <c r="A12" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C12" s="3">
-        <v>40000</v>
-      </c>
-      <c r="D12" s="3">
-        <v>11</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>26</v>
-      </c>
+      <c r="A12" s="4"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
-      <c r="A13" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C13" s="3">
-        <v>40000</v>
-      </c>
-      <c r="D13" s="3">
-        <v>12</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>28</v>
-      </c>
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
-      <c r="A14" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D14" s="3">
-        <v>12</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>32</v>
-      </c>
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
-      <c r="A15" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C15" s="3">
-        <v>40000</v>
-      </c>
-      <c r="D15" s="3">
-        <v>13</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>34</v>
-      </c>
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
-      <c r="A16" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C16" s="3">
-        <v>40000</v>
-      </c>
-      <c r="D16" s="3">
-        <v>14</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>36</v>
-      </c>
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
       <c r="A17" s="4"/>

</xml_diff>

<commit_message>
Adding new logic de FK, START and END Dates
</commit_message>
<xml_diff>
--- a/config/table_config.xlsx
+++ b/config/table_config.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>DOMAIN</t>
   </si>
@@ -41,39 +41,6 @@
   </si>
   <si>
     <t>S_PA0000</t>
-  </si>
-  <si>
-    <t>S_PA0001</t>
-  </si>
-  <si>
-    <t>S_HRP1001</t>
-  </si>
-  <si>
-    <t>OTYPE,OBJID,BEGDA,ENDDA,SCLAS,SOBID,RSIGN,RELAT,PRIOX,PROZT</t>
-  </si>
-  <si>
-    <t>S_INFOTYPE_TEXT</t>
-  </si>
-  <si>
-    <t>INFTY,SUBTY,ENDDA,BEGDA</t>
-  </si>
-  <si>
-    <t>S_PA0006</t>
-  </si>
-  <si>
-    <t>SUBTY,ENDDA,BEGDA,ANSSA,STRAS,ORT01,ORT02,PSTLZ,LAND1,LOCAT,ADR03,ADR04,STATE,HSNMR,BLDNG,FLOOR,STRDS,COUNC,RCTVC,COM01,NUM01,COM02,NUM02,COM03,NUM03,COM04,NUM04,COM05,NUM05,COM06,NUM06</t>
-  </si>
-  <si>
-    <t>S_PA0105</t>
-  </si>
-  <si>
-    <t>PERNR,SUBTY,ENDDA,BEGDA,USRTY</t>
-  </si>
-  <si>
-    <t>S_PA0002</t>
-  </si>
-  <si>
-    <t>PERNR,ENDDA,BEGDA,INITS,NACHN,NACH2,VORNA,TITEL,MIDNM,GESCH,GBDAT,NATIO,SPRSL,FAMST</t>
   </si>
 </sst>
 </file>
@@ -511,7 +478,7 @@
         <v>6</v>
       </c>
       <c r="C2" s="3">
-        <v>2</v>
+        <v>20000</v>
       </c>
       <c r="D2" s="3">
         <v>1</v>
@@ -528,7 +495,7 @@
         <v>8</v>
       </c>
       <c r="C3" s="3">
-        <v>5</v>
+        <v>20000</v>
       </c>
       <c r="D3" s="3">
         <v>2</v>
@@ -536,104 +503,46 @@
       <c r="E3" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
-      <c r="A4" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="3">
-        <v>5</v>
-      </c>
-      <c r="D4" s="3">
-        <v>3</v>
-      </c>
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
       <c r="E4" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
-      <c r="A5" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="3">
-        <v>5</v>
-      </c>
-      <c r="D5" s="3">
-        <v>4</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>11</v>
-      </c>
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
-      <c r="A6" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="3">
-        <v>5</v>
-      </c>
-      <c r="D6" s="3">
-        <v>5</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>13</v>
-      </c>
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
-      <c r="A7" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="3">
-        <v>5</v>
-      </c>
-      <c r="D7" s="3">
-        <v>6</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>15</v>
-      </c>
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
-      <c r="A8" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" s="3">
-        <v>5</v>
-      </c>
-      <c r="D8" s="3">
-        <v>7</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>17</v>
-      </c>
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
-      <c r="A9" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="3">
-        <v>5</v>
-      </c>
-      <c r="D9" s="3">
-        <v>8</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>19</v>
-      </c>
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
       <c r="A10" s="4"/>

</xml_diff>

<commit_message>
Material logic - Changes part 3
</commit_message>
<xml_diff>
--- a/config/table_config.xlsx
+++ b/config/table_config.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="22">
   <si>
     <t>DOMAIN</t>
   </si>
@@ -76,7 +76,10 @@
     <t>S_MBEW_FUTURE</t>
   </si>
   <si>
-    <t/>
+    <t>SAPAPO_MATLSP</t>
+  </si>
+  <si>
+    <t>MARC</t>
   </si>
 </sst>
 </file>
@@ -148,7 +151,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -167,9 +170,6 @@
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
@@ -482,20 +482,20 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="8" width="25.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="8" width="26.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="9" width="20.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="10" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="10" width="141.57642857142858" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="7" width="25.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="7" width="26.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="8" width="20.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="9" width="141.57642857142858" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -512,7 +512,7 @@
         <v>4</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
@@ -520,12 +520,12 @@
         <v>6</v>
       </c>
       <c r="C2" s="5">
-        <v>20</v>
+        <v>20000</v>
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="4" t="s">
         <v>5</v>
       </c>
@@ -533,12 +533,12 @@
         <v>7</v>
       </c>
       <c r="C3" s="5">
-        <v>20</v>
+        <v>20000</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="4" t="s">
         <v>5</v>
       </c>
@@ -546,12 +546,12 @@
         <v>8</v>
       </c>
       <c r="C4" s="5">
-        <v>20</v>
+        <v>20000</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="4" t="s">
         <v>5</v>
       </c>
@@ -559,12 +559,12 @@
         <v>9</v>
       </c>
       <c r="C5" s="5">
-        <v>20</v>
+        <v>20000</v>
       </c>
       <c r="D5" s="5"/>
       <c r="E5" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
@@ -572,12 +572,12 @@
         <v>10</v>
       </c>
       <c r="C6" s="5">
-        <v>20</v>
+        <v>20000</v>
       </c>
       <c r="D6" s="5"/>
       <c r="E6" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="4" t="s">
         <v>5</v>
       </c>
@@ -585,12 +585,12 @@
         <v>11</v>
       </c>
       <c r="C7" s="5">
-        <v>20</v>
+        <v>20000</v>
       </c>
       <c r="D7" s="5"/>
       <c r="E7" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="4" t="s">
         <v>5</v>
       </c>
@@ -598,12 +598,12 @@
         <v>12</v>
       </c>
       <c r="C8" s="5">
-        <v>20</v>
+        <v>20000</v>
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="4" t="s">
         <v>5</v>
       </c>
@@ -611,12 +611,12 @@
         <v>13</v>
       </c>
       <c r="C9" s="5">
-        <v>20</v>
+        <v>20000</v>
       </c>
       <c r="D9" s="5"/>
       <c r="E9" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="4" t="s">
         <v>5</v>
       </c>
@@ -624,12 +624,12 @@
         <v>14</v>
       </c>
       <c r="C10" s="5">
-        <v>20</v>
+        <v>20000</v>
       </c>
       <c r="D10" s="5"/>
       <c r="E10" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="4" t="s">
         <v>5</v>
       </c>
@@ -637,12 +637,12 @@
         <v>15</v>
       </c>
       <c r="C11" s="5">
-        <v>20</v>
+        <v>20000</v>
       </c>
       <c r="D11" s="5"/>
       <c r="E11" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="4" t="s">
         <v>5</v>
       </c>
@@ -650,12 +650,12 @@
         <v>16</v>
       </c>
       <c r="C12" s="5">
-        <v>20</v>
-      </c>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18">
+        <v>20000</v>
+      </c>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="4" t="s">
         <v>5</v>
       </c>
@@ -663,12 +663,12 @@
         <v>17</v>
       </c>
       <c r="C13" s="5">
-        <v>20</v>
-      </c>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18">
+        <v>20000</v>
+      </c>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
       <c r="A14" s="4" t="s">
         <v>5</v>
       </c>
@@ -676,12 +676,12 @@
         <v>18</v>
       </c>
       <c r="C14" s="5">
-        <v>20</v>
-      </c>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18">
+        <v>20000</v>
+      </c>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
       <c r="A15" s="4" t="s">
         <v>5</v>
       </c>
@@ -689,21 +689,36 @@
         <v>19</v>
       </c>
       <c r="C15" s="5">
+        <v>20000</v>
+      </c>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="17.25">
+      <c r="A16" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
-      <c r="A16" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="3"/>
+      <c r="C16" s="5">
+        <v>20000</v>
+      </c>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
+      <c r="A17" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" s="5">
+        <v>20000</v>
+      </c>
+      <c r="D17" s="5"/>
+      <c r="E17" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>